<commit_message>
Version compliada y funcional FrontEnd Gastos Diarios
</commit_message>
<xml_diff>
--- a/exports/Reporte.xlsx
+++ b/exports/Reporte.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="157">
   <si>
     <t>Accounts</t>
   </si>
@@ -102,6 +102,393 @@
   </si>
   <si>
     <t>Symbol</t>
+  </si>
+  <si>
+    <t>AED</t>
+  </si>
+  <si>
+    <t>د.إ</t>
+  </si>
+  <si>
+    <t>AFS</t>
+  </si>
+  <si>
+    <t>Af</t>
+  </si>
+  <si>
+    <t>AKZ</t>
+  </si>
+  <si>
+    <t>Kz</t>
+  </si>
+  <si>
+    <t>ARS</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>AUD</t>
+  </si>
+  <si>
+    <t>AZN</t>
+  </si>
+  <si>
+    <t>ман.</t>
+  </si>
+  <si>
+    <t>BAM</t>
+  </si>
+  <si>
+    <t>KM</t>
+  </si>
+  <si>
+    <t>BDT</t>
+  </si>
+  <si>
+    <t>৳</t>
+  </si>
+  <si>
+    <t>BGN</t>
+  </si>
+  <si>
+    <t>лв.</t>
+  </si>
+  <si>
+    <t>BHD</t>
+  </si>
+  <si>
+    <t>.د.ب</t>
+  </si>
+  <si>
+    <t>BOB</t>
+  </si>
+  <si>
+    <t>Bs.</t>
+  </si>
+  <si>
+    <t>BRL</t>
+  </si>
+  <si>
+    <t>R$</t>
+  </si>
+  <si>
+    <t>BTC</t>
+  </si>
+  <si>
+    <t>Ƀ</t>
+  </si>
+  <si>
+    <t>CAD</t>
+  </si>
+  <si>
+    <t>C$</t>
+  </si>
+  <si>
+    <t>CHF</t>
+  </si>
+  <si>
+    <t>Fr.</t>
+  </si>
+  <si>
+    <t>CLP</t>
+  </si>
+  <si>
+    <t>CNY</t>
+  </si>
+  <si>
+    <t>¥</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>CRC</t>
+  </si>
+  <si>
+    <t>₡</t>
+  </si>
+  <si>
+    <t>CZK</t>
+  </si>
+  <si>
+    <t>Kč</t>
+  </si>
+  <si>
+    <t>DKK</t>
+  </si>
+  <si>
+    <t>kr</t>
+  </si>
+  <si>
+    <t>DOP</t>
+  </si>
+  <si>
+    <t>RD$</t>
+  </si>
+  <si>
+    <t>EGP</t>
+  </si>
+  <si>
+    <t>ج.م</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>â‚¬</t>
+  </si>
+  <si>
+    <t>GBP</t>
+  </si>
+  <si>
+    <t>£</t>
+  </si>
+  <si>
+    <t>GTQ</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>HKD</t>
+  </si>
+  <si>
+    <t>HNL</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>HRK</t>
+  </si>
+  <si>
+    <t>kn</t>
+  </si>
+  <si>
+    <t>HUF</t>
+  </si>
+  <si>
+    <t>Ft</t>
+  </si>
+  <si>
+    <t>IDR</t>
+  </si>
+  <si>
+    <t>Rp</t>
+  </si>
+  <si>
+    <t>ILS</t>
+  </si>
+  <si>
+    <t>₪</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>₹</t>
+  </si>
+  <si>
+    <t>JPY</t>
+  </si>
+  <si>
+    <t>KES</t>
+  </si>
+  <si>
+    <t>KSh</t>
+  </si>
+  <si>
+    <t>KRW</t>
+  </si>
+  <si>
+    <t>₩</t>
+  </si>
+  <si>
+    <t>KWD</t>
+  </si>
+  <si>
+    <t>د.ك</t>
+  </si>
+  <si>
+    <t>KZT</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>LBP</t>
+  </si>
+  <si>
+    <t>ل.ل.</t>
+  </si>
+  <si>
+    <t>LKR</t>
+  </si>
+  <si>
+    <t>Rs</t>
+  </si>
+  <si>
+    <t>MAD</t>
+  </si>
+  <si>
+    <t>درهم</t>
+  </si>
+  <si>
+    <t>MXN</t>
+  </si>
+  <si>
+    <t>MYR</t>
+  </si>
+  <si>
+    <t>RM</t>
+  </si>
+  <si>
+    <t>NGN</t>
+  </si>
+  <si>
+    <t>₦</t>
+  </si>
+  <si>
+    <t>NIO</t>
+  </si>
+  <si>
+    <t>NOK</t>
+  </si>
+  <si>
+    <t>NZD</t>
+  </si>
+  <si>
+    <t>OMR</t>
+  </si>
+  <si>
+    <t>ر.ع.</t>
+  </si>
+  <si>
+    <t>PAB</t>
+  </si>
+  <si>
+    <t>PEN</t>
+  </si>
+  <si>
+    <t>S/.</t>
+  </si>
+  <si>
+    <t>PHP</t>
+  </si>
+  <si>
+    <t>₱</t>
+  </si>
+  <si>
+    <t>PKR</t>
+  </si>
+  <si>
+    <t>PLN</t>
+  </si>
+  <si>
+    <t>zł</t>
+  </si>
+  <si>
+    <t>PYG</t>
+  </si>
+  <si>
+    <t>Gs.</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>lei</t>
+  </si>
+  <si>
+    <t>RUB</t>
+  </si>
+  <si>
+    <t>₽</t>
+  </si>
+  <si>
+    <t>RWF</t>
+  </si>
+  <si>
+    <t>R₣</t>
+  </si>
+  <si>
+    <t>SAR</t>
+  </si>
+  <si>
+    <t>ر.س</t>
+  </si>
+  <si>
+    <t>SEK</t>
+  </si>
+  <si>
+    <t>SGD</t>
+  </si>
+  <si>
+    <t>SVC</t>
+  </si>
+  <si>
+    <t>THB</t>
+  </si>
+  <si>
+    <t>฿</t>
+  </si>
+  <si>
+    <t>TND</t>
+  </si>
+  <si>
+    <t>د.ت</t>
+  </si>
+  <si>
+    <t>TRY</t>
+  </si>
+  <si>
+    <t>₺</t>
+  </si>
+  <si>
+    <t>TWD</t>
+  </si>
+  <si>
+    <t>TZS</t>
+  </si>
+  <si>
+    <t>Tsh</t>
+  </si>
+  <si>
+    <t>UAH</t>
+  </si>
+  <si>
+    <t>₴</t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t>UYU</t>
+  </si>
+  <si>
+    <t>$U</t>
+  </si>
+  <si>
+    <t>VEF</t>
+  </si>
+  <si>
+    <t>VND</t>
+  </si>
+  <si>
+    <t>₫</t>
+  </si>
+  <si>
+    <t>XOF</t>
+  </si>
+  <si>
+    <t>CFA</t>
+  </si>
+  <si>
+    <t>ZAR</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
   <si>
     <t>Movements</t>
@@ -932,7 +1319,7 @@
   <sheetPr filterMode="1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C77"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -968,7 +1355,590 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" customHeight="1" ht="24.95"/>
+    <row r="5" spans="1:3" customHeight="1" ht="25">
+      <c r="A5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" customHeight="1" ht="25">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" customHeight="1" ht="25">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" customHeight="1" ht="25">
+      <c r="A8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" customHeight="1" ht="25">
+      <c r="A9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" customHeight="1" ht="25">
+      <c r="A10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" customHeight="1" ht="25">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" customHeight="1" ht="25">
+      <c r="A12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" customHeight="1" ht="25">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" customHeight="1" ht="25">
+      <c r="A14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" customHeight="1" ht="25">
+      <c r="A15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" customHeight="1" ht="25">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" customHeight="1" ht="25">
+      <c r="A17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" customHeight="1" ht="25">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" customHeight="1" ht="25">
+      <c r="A19" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" customHeight="1" ht="25">
+      <c r="A20" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" customHeight="1" ht="25">
+      <c r="A21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" customHeight="1" ht="25">
+      <c r="A22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" customHeight="1" ht="25">
+      <c r="A23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" customHeight="1" ht="25">
+      <c r="A24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" customHeight="1" ht="25">
+      <c r="A25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" customHeight="1" ht="25">
+      <c r="A26" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" customHeight="1" ht="25">
+      <c r="A27" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" customHeight="1" ht="25">
+      <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" customHeight="1" ht="25">
+      <c r="A29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" customHeight="1" ht="25">
+      <c r="A30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" customHeight="1" ht="25">
+      <c r="A31" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" customHeight="1" ht="25">
+      <c r="A32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" customHeight="1" ht="25">
+      <c r="A33" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" customHeight="1" ht="25">
+      <c r="A34" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" customHeight="1" ht="25">
+      <c r="A35" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" customHeight="1" ht="25">
+      <c r="A36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" customHeight="1" ht="25">
+      <c r="A37" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" customHeight="1" ht="25">
+      <c r="A38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" customHeight="1" ht="25">
+      <c r="A39" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" customHeight="1" ht="25">
+      <c r="A40" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" customHeight="1" ht="25">
+      <c r="A41" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" customHeight="1" ht="25">
+      <c r="A42" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" customHeight="1" ht="25">
+      <c r="A43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" customHeight="1" ht="25">
+      <c r="A44" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" customHeight="1" ht="25">
+      <c r="A45" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" customHeight="1" ht="25">
+      <c r="A46" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" customHeight="1" ht="25">
+      <c r="A47" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" customHeight="1" ht="25">
+      <c r="A48" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" customHeight="1" ht="25">
+      <c r="A49" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" customHeight="1" ht="25">
+      <c r="A50" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" customHeight="1" ht="25">
+      <c r="A51" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" customHeight="1" ht="25">
+      <c r="A52" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" customHeight="1" ht="25">
+      <c r="A53" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" customHeight="1" ht="25">
+      <c r="A54" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" customHeight="1" ht="25">
+      <c r="A55" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" customHeight="1" ht="25">
+      <c r="A56" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" customHeight="1" ht="25">
+      <c r="A57" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" customHeight="1" ht="25">
+      <c r="A58" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" customHeight="1" ht="25">
+      <c r="A59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" customHeight="1" ht="25">
+      <c r="A60" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" customHeight="1" ht="25">
+      <c r="A61" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" customHeight="1" ht="25">
+      <c r="A62" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" customHeight="1" ht="25">
+      <c r="A63" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" customHeight="1" ht="25">
+      <c r="A64" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" customHeight="1" ht="25">
+      <c r="A65" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" customHeight="1" ht="25">
+      <c r="A66" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" customHeight="1" ht="25">
+      <c r="A67" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" customHeight="1" ht="25">
+      <c r="A68" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" customHeight="1" ht="25">
+      <c r="A69" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" customHeight="1" ht="25">
+      <c r="A70" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" customHeight="1" ht="25">
+      <c r="A71" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" customHeight="1" ht="25">
+      <c r="A72" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" customHeight="1" ht="25">
+      <c r="A73" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" customHeight="1" ht="25">
+      <c r="A74" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" customHeight="1" ht="25">
+      <c r="A75" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" customHeight="1" ht="25">
+      <c r="A76" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" customHeight="1" ht="25">
+      <c r="A77" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <autoFilter ref="A4:B4"/>
@@ -1015,7 +1985,7 @@
   <sheetData>
     <row r="1" spans="1:8" customHeight="1" ht="24.95" s="6" customFormat="1">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>154</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1059,10 +2029,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>26</v>
+        <v>155</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>27</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:8" customHeight="1" ht="24.95"/>

</xml_diff>